<commit_message>
Development of a new RW algorithm
</commit_message>
<xml_diff>
--- a/Алгоритмы и описание/RailWay/Описания полей RW.xlsx
+++ b/Алгоритмы и описание/RailWay/Описания полей RW.xlsx
@@ -5,14 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Мои документы\Visual Studio 2013\Projects\Work\New RailWay\Documents\Алгоритмы\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work MPP\Логистика\RailWay\RW_Documents\Алгоритмы и описание\RailWay\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cars" sheetId="1" r:id="rId1"/>
+    <sheet name="CarsInternal" sheetId="2" r:id="rId2"/>
+    <sheet name="CarOperations" sheetId="3" r:id="rId3"/>
+    <sheet name="CarInboundDelivery" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="87">
   <si>
     <t>id</t>
   </si>
@@ -138,6 +141,153 @@
   </si>
   <si>
     <t>Пустое</t>
+  </si>
+  <si>
+    <t>natur_kis_inp</t>
+  </si>
+  <si>
+    <t>natur_rw</t>
+  </si>
+  <si>
+    <t>id_car_internal</t>
+  </si>
+  <si>
+    <t>id_car_conditions</t>
+  </si>
+  <si>
+    <t>id_car_status</t>
+  </si>
+  <si>
+    <t>dt_inp</t>
+  </si>
+  <si>
+    <t>dt_out</t>
+  </si>
+  <si>
+    <t>id_way</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>train1</t>
+  </si>
+  <si>
+    <t>train2</t>
+  </si>
+  <si>
+    <t>side</t>
+  </si>
+  <si>
+    <t>user_edit</t>
+  </si>
+  <si>
+    <t>dt_edit</t>
+  </si>
+  <si>
+    <t>composition_index</t>
+  </si>
+  <si>
+    <t>num_car</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>nvarchar(250)</t>
+  </si>
+  <si>
+    <t>num_nakl_sap</t>
+  </si>
+  <si>
+    <t>nvarchar(35)</t>
+  </si>
+  <si>
+    <t>country_code</t>
+  </si>
+  <si>
+    <t>id_country</t>
+  </si>
+  <si>
+    <t>weight_cargo</t>
+  </si>
+  <si>
+    <t>numeric(18, 3)</t>
+  </si>
+  <si>
+    <t>num_doc_reweighing_sap</t>
+  </si>
+  <si>
+    <t>dt_doc_reweighing_sap</t>
+  </si>
+  <si>
+    <t>weight_reweighing_sap</t>
+  </si>
+  <si>
+    <t>dt_reweighing_sap</t>
+  </si>
+  <si>
+    <t>post_reweighing_sap</t>
+  </si>
+  <si>
+    <t>cargo_code</t>
+  </si>
+  <si>
+    <t>id_cargo</t>
+  </si>
+  <si>
+    <t>material_code_sap</t>
+  </si>
+  <si>
+    <t>nvarchar(18)</t>
+  </si>
+  <si>
+    <t>material_name_sap</t>
+  </si>
+  <si>
+    <t>station_shipment</t>
+  </si>
+  <si>
+    <t>station_shipment_code_sap</t>
+  </si>
+  <si>
+    <t>nvarchar(3)</t>
+  </si>
+  <si>
+    <t>station_shipment_name_sap</t>
+  </si>
+  <si>
+    <t>consignee</t>
+  </si>
+  <si>
+    <t>id_consignee</t>
+  </si>
+  <si>
+    <t>shop_code_sap</t>
+  </si>
+  <si>
+    <t>nvarchar(4)</t>
+  </si>
+  <si>
+    <t>shop_name_sap</t>
+  </si>
+  <si>
+    <t>new_shop_code_sap</t>
+  </si>
+  <si>
+    <t>new_shop_name_sap</t>
+  </si>
+  <si>
+    <t>permission_unload_sap</t>
+  </si>
+  <si>
+    <t>bit</t>
+  </si>
+  <si>
+    <t>step1_sap</t>
+  </si>
+  <si>
+    <t>step2_sap</t>
   </si>
 </sst>
 </file>
@@ -217,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -229,6 +379,11 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -516,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,4 +901,765 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>86</v>
+      </c>
+      <c r="B34" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>